<commit_message>
Page read order introduced
Pages can now be associated with a read order, default 0 in settings page specs, that determines which page gets read in first for a workbook.
By settings the transition page as 1, it now gets read after the parameters page, even if positioned beforehand, thus allowing parameter definitional order to be maintained.
Accordingly, dependencies are marked appropriately and the TB test case now has a stable population size, with FOI calculated as zero.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAA7A06-10BA-4175-9A4D-945FBCA3F44C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8333D8B-41A9-470A-8C8A-F412B6CCA3A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4893,16 +4893,16 @@
     <t>OR</t>
   </si>
   <si>
+    <t>Number of births</t>
+  </si>
+  <si>
     <t>Non-TB death rate</t>
   </si>
   <si>
-    <t>Emigration rate</t>
+    <t>Number of new immigrants</t>
   </si>
   <si>
-    <t>Number of births</t>
-  </si>
-  <si>
-    <t>Number of new immigrants</t>
+    <t>Emigration rate</t>
   </si>
   <si>
     <t>Known SP drug-susceptible infections</t>
@@ -4992,12 +4992,6 @@
     <t>XDR proportion of new SN infections</t>
   </si>
   <si>
-    <t>Reactivation rate for recovered active cases</t>
-  </si>
-  <si>
-    <t>Probability</t>
-  </si>
-  <si>
     <t>Infection vulnerability factor (vaccinated versus susceptible)</t>
   </si>
   <si>
@@ -5017,6 +5011,12 @@
   </si>
   <si>
     <t>Relative infectiousness (XDR versus DS)</t>
+  </si>
+  <si>
+    <t>Reactivation rate for recovered active cases</t>
+  </si>
+  <si>
+    <t>Probability</t>
   </si>
   <si>
     <t>Vaccinated</t>
@@ -5145,13 +5145,7 @@
     <t>DS-SP natural recovery rate</t>
   </si>
   <si>
-    <t>SP DS-MDR escalation rate via improper treatment</t>
-  </si>
-  <si>
     <t>MDR-SP natural recovery rate</t>
-  </si>
-  <si>
-    <t>SP MDR-XDR escalation rate via improper treatment</t>
   </si>
   <si>
     <t>XDR-SP natural recovery rate</t>
@@ -5160,31 +5154,37 @@
     <t>DS-SN natural recovery rate</t>
   </si>
   <si>
-    <t>SN DS-MDR escalation rate via improper treatment</t>
+    <t>MDR-SN natural recovery rate</t>
   </si>
   <si>
-    <t>MDR-SN natural recovery rate</t>
+    <t>XDR-SN natural recovery rate</t>
+  </si>
+  <si>
+    <t>SN DS-MDR escalation rate via improper treatment</t>
   </si>
   <si>
     <t>SN MDR-XDR escalation rate via improper treatment</t>
   </si>
   <si>
-    <t>XDR-SN natural recovery rate</t>
+    <t>SP DS-MDR escalation rate via improper treatment</t>
+  </si>
+  <si>
+    <t>SP MDR-XDR escalation rate via improper treatment</t>
   </si>
   <si>
     <t>DS-SP death rate (untreated)</t>
   </si>
   <si>
+    <t>MDR-SP death rate (untreated)</t>
+  </si>
+  <si>
+    <t>XDR-SP death rate (untreated)</t>
+  </si>
+  <si>
     <t>DS-SP death rate (treated)</t>
   </si>
   <si>
-    <t>MDR-SP death rate (untreated)</t>
-  </si>
-  <si>
     <t>MDR-SP death rate (treated)</t>
-  </si>
-  <si>
-    <t>XDR-SP death rate (untreated)</t>
   </si>
   <si>
     <t>XDR-SP death rate (treated)</t>
@@ -5193,16 +5193,16 @@
     <t>DS-SN death rate (untreated)</t>
   </si>
   <si>
+    <t>MDR-SN death rate (untreated)</t>
+  </si>
+  <si>
+    <t>XDR-SN death rate (untreated)</t>
+  </si>
+  <si>
     <t>DS-SN death rate (treated)</t>
   </si>
   <si>
-    <t>MDR-SN death rate (untreated)</t>
-  </si>
-  <si>
     <t>MDR-SN death rate (treated)</t>
-  </si>
-  <si>
-    <t>XDR-SN death rate (untreated)</t>
   </si>
   <si>
     <t>XDR-SN death rate (treated)</t>
@@ -16584,8 +16584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16679,10 +16679,10 @@
         <v>48</v>
       </c>
       <c r="E2" s="3">
-        <v>9000000</v>
+        <v>500000</v>
       </c>
       <c r="O2" s="3">
-        <v>11000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.45">
@@ -17525,25 +17525,25 @@
       <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0200-000007000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{00000000-0002-0000-0200-000008000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{00000000-0002-0000-0200-000009000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0200-00000A000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0200-00000B000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0200-00000C000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0200-00000D000000}">
-      <formula1>"Number,Probability"</formula1>
+      <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0200-00000E000000}">
       <formula1>"Number,Probability"</formula1>
@@ -17588,25 +17588,25 @@
       <formula1>"Number"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38" xr:uid="{00000000-0002-0000-0200-00001C000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39" xr:uid="{00000000-0002-0000-0200-00001D000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40" xr:uid="{00000000-0002-0000-0200-00001E000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41" xr:uid="{00000000-0002-0000-0200-00001F000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{00000000-0002-0000-0200-000020000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43" xr:uid="{00000000-0002-0000-0200-000021000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{00000000-0002-0000-0200-000022000000}">
-      <formula1>"Number"</formula1>
+      <formula1>"Number,Probability"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23572,7 +23572,7 @@
         <v>Population 0</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:C17" si="1">IF(SUMPRODUCT(--(E11:W11&lt;&gt;""))=0,0,"N.A.")</f>
@@ -23588,7 +23588,7 @@
         <v>Population 1</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -23604,7 +23604,7 @@
         <v>Population 2</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -23620,7 +23620,7 @@
         <v>Population 3</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -23636,7 +23636,7 @@
         <v>Population 4</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -23652,7 +23652,7 @@
         <v>Population 5</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -23668,7 +23668,7 @@
         <v>Population 6</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -23680,7 +23680,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>45</v>
@@ -23752,7 +23752,7 @@
         <v>Population 0</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:C26" si="2">IF(SUMPRODUCT(--(E20:W20&lt;&gt;""))=0,0,"N.A.")</f>
@@ -23768,7 +23768,7 @@
         <v>Population 1</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
@@ -23784,7 +23784,7 @@
         <v>Population 2</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
@@ -23800,7 +23800,7 @@
         <v>Population 3</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
@@ -23816,7 +23816,7 @@
         <v>Population 4</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
@@ -23832,7 +23832,7 @@
         <v>Population 5</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
@@ -23848,7 +23848,7 @@
         <v>Population 6</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
@@ -23860,7 +23860,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
@@ -23932,7 +23932,7 @@
         <v>Population 0</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:C35" si="3">IF(SUMPRODUCT(--(E29:W29&lt;&gt;""))=0,0,"N.A.")</f>
@@ -23948,7 +23948,7 @@
         <v>Population 1</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <f t="shared" si="3"/>
@@ -23964,7 +23964,7 @@
         <v>Population 2</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31">
         <f t="shared" si="3"/>
@@ -23980,7 +23980,7 @@
         <v>Population 3</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <f t="shared" si="3"/>
@@ -23996,7 +23996,7 @@
         <v>Population 4</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33">
         <f t="shared" si="3"/>
@@ -24012,7 +24012,7 @@
         <v>Population 5</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <f t="shared" si="3"/>
@@ -24028,7 +24028,7 @@
         <v>Population 6</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <f t="shared" si="3"/>
@@ -24040,7 +24040,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>45</v>
@@ -24112,7 +24112,7 @@
         <v>Population 0</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C44" si="4">IF(SUMPRODUCT(--(E38:W38&lt;&gt;""))=0,0,"N.A.")</f>
@@ -24128,7 +24128,7 @@
         <v>Population 1</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <f t="shared" si="4"/>
@@ -24144,7 +24144,7 @@
         <v>Population 2</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40">
         <f t="shared" si="4"/>
@@ -24160,7 +24160,7 @@
         <v>Population 3</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <f t="shared" si="4"/>
@@ -24176,7 +24176,7 @@
         <v>Population 4</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <f t="shared" si="4"/>
@@ -24192,7 +24192,7 @@
         <v>Population 5</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43">
         <f t="shared" si="4"/>
@@ -24208,7 +24208,7 @@
         <v>Population 6</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44">
         <f t="shared" si="4"/>
@@ -24220,7 +24220,7 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
@@ -24292,7 +24292,7 @@
         <v>Population 0</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47">
         <f t="shared" ref="C47:C53" si="5">IF(SUMPRODUCT(--(E47:W47&lt;&gt;""))=0,0,"N.A.")</f>
@@ -24308,7 +24308,7 @@
         <v>Population 1</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C48">
         <f t="shared" si="5"/>
@@ -24324,7 +24324,7 @@
         <v>Population 2</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49">
         <f t="shared" si="5"/>
@@ -24340,7 +24340,7 @@
         <v>Population 3</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C50">
         <f t="shared" si="5"/>
@@ -24356,7 +24356,7 @@
         <v>Population 4</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <f t="shared" si="5"/>
@@ -24372,7 +24372,7 @@
         <v>Population 5</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52">
         <f t="shared" si="5"/>
@@ -24388,7 +24388,7 @@
         <v>Population 6</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C53">
         <f t="shared" si="5"/>
@@ -24400,7 +24400,7 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>45</v>
@@ -24472,7 +24472,7 @@
         <v>Population 0</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C56">
         <f t="shared" ref="C56:C62" si="6">IF(SUMPRODUCT(--(E56:W56&lt;&gt;""))=0,0,"N.A.")</f>
@@ -24488,7 +24488,7 @@
         <v>Population 1</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C57">
         <f t="shared" si="6"/>
@@ -24504,7 +24504,7 @@
         <v>Population 2</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C58">
         <f t="shared" si="6"/>
@@ -24520,7 +24520,7 @@
         <v>Population 3</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C59">
         <f t="shared" si="6"/>
@@ -24536,7 +24536,7 @@
         <v>Population 4</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C60">
         <f t="shared" si="6"/>
@@ -24552,7 +24552,7 @@
         <v>Population 5</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C61">
         <f t="shared" si="6"/>
@@ -24568,7 +24568,7 @@
         <v>Population 6</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C62">
         <f t="shared" si="6"/>
@@ -24581,25 +24581,25 @@
   </sheetData>
   <dataValidations count="49">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0600-000000000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0600-000001000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0600-000002000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0600-000003000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0600-000004000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0600-000005000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0600-000006000000}">
-      <formula1>"Probability"</formula1>
+      <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0600-000007000000}">
       <formula1>"N.A."</formula1>
@@ -24707,25 +24707,25 @@
       <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56" xr:uid="{00000000-0002-0000-0600-00002A000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{00000000-0002-0000-0600-00002B000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58" xr:uid="{00000000-0002-0000-0600-00002C000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{00000000-0002-0000-0600-00002D000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60" xr:uid="{00000000-0002-0000-0600-00002E000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61" xr:uid="{00000000-0002-0000-0600-00002F000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62" xr:uid="{00000000-0002-0000-0600-000030000000}">
-      <formula1>"N.A."</formula1>
+      <formula1>"Probability"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25540,7 +25540,7 @@
         <v>Population 0</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C44" si="4">IF(SUMPRODUCT(--(E38:W38&lt;&gt;""))=0,0,"N.A.")</f>
@@ -25556,7 +25556,7 @@
         <v>Population 1</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <f t="shared" si="4"/>
@@ -25572,7 +25572,7 @@
         <v>Population 2</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40">
         <f t="shared" si="4"/>
@@ -25588,7 +25588,7 @@
         <v>Population 3</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <f t="shared" si="4"/>
@@ -25604,7 +25604,7 @@
         <v>Population 4</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <f t="shared" si="4"/>
@@ -25620,7 +25620,7 @@
         <v>Population 5</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43">
         <f t="shared" si="4"/>
@@ -25636,7 +25636,7 @@
         <v>Population 6</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44">
         <f t="shared" si="4"/>
@@ -25720,7 +25720,7 @@
         <v>Population 0</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47">
         <f t="shared" ref="C47:C53" si="5">IF(SUMPRODUCT(--(E47:W47&lt;&gt;""))=0,0,"N.A.")</f>
@@ -25736,7 +25736,7 @@
         <v>Population 1</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C48">
         <f t="shared" si="5"/>
@@ -25752,7 +25752,7 @@
         <v>Population 2</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49">
         <f t="shared" si="5"/>
@@ -25768,7 +25768,7 @@
         <v>Population 3</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C50">
         <f t="shared" si="5"/>
@@ -25784,7 +25784,7 @@
         <v>Population 4</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <f t="shared" si="5"/>
@@ -25800,7 +25800,7 @@
         <v>Population 5</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52">
         <f t="shared" si="5"/>
@@ -25816,7 +25816,7 @@
         <v>Population 6</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C53">
         <f t="shared" si="5"/>
@@ -25900,7 +25900,7 @@
         <v>Population 0</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C56">
         <f t="shared" ref="C56:C62" si="6">IF(SUMPRODUCT(--(E56:W56&lt;&gt;""))=0,0,"N.A.")</f>
@@ -25916,7 +25916,7 @@
         <v>Population 1</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C57">
         <f t="shared" si="6"/>
@@ -25932,7 +25932,7 @@
         <v>Population 2</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C58">
         <f t="shared" si="6"/>
@@ -25948,7 +25948,7 @@
         <v>Population 3</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C59">
         <f t="shared" si="6"/>
@@ -25964,7 +25964,7 @@
         <v>Population 4</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C60">
         <f t="shared" si="6"/>
@@ -25980,7 +25980,7 @@
         <v>Population 5</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C61">
         <f t="shared" si="6"/>
@@ -25996,7 +25996,7 @@
         <v>Population 6</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C62">
         <f t="shared" si="6"/>
@@ -26248,7 +26248,7 @@
         <v>Population 0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C8" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
@@ -26264,7 +26264,7 @@
         <v>Population 1</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
@@ -26280,7 +26280,7 @@
         <v>Population 2</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -26296,7 +26296,7 @@
         <v>Population 3</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -26312,7 +26312,7 @@
         <v>Population 4</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -26328,7 +26328,7 @@
         <v>Population 5</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -26344,7 +26344,7 @@
         <v>Population 6</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -26428,7 +26428,7 @@
         <v>Population 0</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:C17" si="1">IF(SUMPRODUCT(--(E11:W11&lt;&gt;""))=0,0,"N.A.")</f>
@@ -26444,7 +26444,7 @@
         <v>Population 1</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -26460,7 +26460,7 @@
         <v>Population 2</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -26476,7 +26476,7 @@
         <v>Population 3</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -26492,7 +26492,7 @@
         <v>Population 4</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -26508,7 +26508,7 @@
         <v>Population 5</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -26524,7 +26524,7 @@
         <v>Population 6</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -26608,7 +26608,7 @@
         <v>Population 0</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:C26" si="2">IF(SUMPRODUCT(--(E20:W20&lt;&gt;""))=0,0,"N.A.")</f>
@@ -26624,7 +26624,7 @@
         <v>Population 1</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
@@ -26640,7 +26640,7 @@
         <v>Population 2</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
@@ -26656,7 +26656,7 @@
         <v>Population 3</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
@@ -26672,7 +26672,7 @@
         <v>Population 4</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
@@ -26688,7 +26688,7 @@
         <v>Population 5</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
@@ -26704,7 +26704,7 @@
         <v>Population 6</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Pop links successfully parsed
Transfer items and related connections are successfully being read from the TB test databook.
TDVE tables now need to be constructed specially for transfers.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AD3144-0414-4804-9523-50ABAF60DFAA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A4E862-BD22-4EA6-AF1A-C38E200743F7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4802,7 +4802,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="213">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -5407,18 +5407,6 @@
     <t>MDR-SP treatment success rate</t>
   </si>
   <si>
-    <t>trans_0</t>
-  </si>
-  <si>
-    <t>Transfer 0</t>
-  </si>
-  <si>
-    <t>trans_1</t>
-  </si>
-  <si>
-    <t>Transfer 1</t>
-  </si>
-  <si>
     <t>trans_2</t>
   </si>
   <si>
@@ -5438,6 +5426,21 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Aging</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>HIV Infection</t>
+  </si>
+  <si>
+    <t>trans_hiv</t>
+  </si>
+  <si>
+    <t>trans_age</t>
   </si>
 </sst>
 </file>
@@ -27245,14 +27248,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A99255-0B6D-41A7-8133-CB3A9221CAB5}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="143" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" style="143" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="143" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" style="143" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" style="143" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.06640625" style="143" bestFit="1" customWidth="1"/>
@@ -27277,48 +27280,48 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="48" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="48" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="48" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="48" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="48" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="str">
         <f>$B$2</f>
-        <v>Transfer 0</v>
+        <v>Aging</v>
       </c>
       <c r="B8" s="163" t="str">
         <f>'Population Definitions'!$A$2</f>
@@ -27378,37 +27381,37 @@
         <v>103</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M9" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -27417,40 +27420,40 @@
         <v>5-14</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C10" s="48" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M10" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
@@ -27459,40 +27462,40 @@
         <v>15-64</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M11" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -27501,40 +27504,40 @@
         <v>65+</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E12" s="48" t="s">
         <v>103</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M12" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -27543,40 +27546,40 @@
         <v>15-64 (HIV+)</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>103</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M13" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
@@ -27585,40 +27588,40 @@
         <v>65+ (HIV+)</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>103</v>
       </c>
       <c r="H14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M14" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
@@ -27627,40 +27630,40 @@
         <v>Pris</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>103</v>
       </c>
       <c r="I15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M15" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
@@ -27669,40 +27672,40 @@
         <v>Pris (HIV+)</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I16" s="48" t="s">
         <v>103</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M16" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
@@ -27711,40 +27714,40 @@
         <v>HCW</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J17" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M17" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
@@ -27753,40 +27756,40 @@
         <v>HCW (HIV+)</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K18" s="48" t="s">
         <v>103</v>
       </c>
       <c r="L18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M18" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
@@ -27795,40 +27798,40 @@
         <v>Mine</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L19" s="48" t="s">
         <v>103</v>
       </c>
       <c r="M19" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
@@ -27837,37 +27840,37 @@
         <v>Mine (HIV+)</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L20" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M20" s="48" t="s">
         <v>103</v>
@@ -27876,7 +27879,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="str">
         <f>$B$3</f>
-        <v>Transfer 1</v>
+        <v>HIV Infection</v>
       </c>
       <c r="B22" s="163" t="str">
         <f>'Population Definitions'!$A$2</f>
@@ -27936,37 +27939,37 @@
         <v>103</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M23" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
@@ -27975,40 +27978,40 @@
         <v>5-14</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C24" s="48" t="s">
         <v>103</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M24" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
@@ -28017,40 +28020,40 @@
         <v>15-64</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D25" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M25" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
@@ -28059,40 +28062,40 @@
         <v>65+</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E26" s="48" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G26" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M26" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
@@ -28101,40 +28104,40 @@
         <v>15-64 (HIV+)</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>103</v>
       </c>
       <c r="G27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M27" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
@@ -28143,40 +28146,40 @@
         <v>65+ (HIV+)</v>
       </c>
       <c r="B28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G28" s="48" t="s">
         <v>103</v>
       </c>
       <c r="H28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M28" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
@@ -28185,40 +28188,40 @@
         <v>Pris</v>
       </c>
       <c r="B29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H29" s="48" t="s">
         <v>103</v>
       </c>
       <c r="I29" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M29" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.45">
@@ -28227,40 +28230,40 @@
         <v>Pris (HIV+)</v>
       </c>
       <c r="B30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I30" s="48" t="s">
         <v>103</v>
       </c>
       <c r="J30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M30" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.45">
@@ -28269,40 +28272,40 @@
         <v>HCW</v>
       </c>
       <c r="B31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J31" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K31" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.45">
@@ -28311,40 +28314,40 @@
         <v>HCW (HIV+)</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>103</v>
       </c>
       <c r="L32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.45">
@@ -28353,40 +28356,40 @@
         <v>Mine</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K33" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L33" s="48" t="s">
         <v>103</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.45">
@@ -28395,37 +28398,37 @@
         <v>Mine (HIV+)</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L34" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M34" s="48" t="s">
         <v>103</v>
@@ -28494,37 +28497,37 @@
         <v>103</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M37" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
@@ -28533,40 +28536,40 @@
         <v>5-14</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C38" s="48" t="s">
         <v>103</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M38" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.45">
@@ -28575,40 +28578,40 @@
         <v>15-64</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D39" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M39" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.45">
@@ -28617,40 +28620,40 @@
         <v>65+</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E40" s="48" t="s">
         <v>103</v>
       </c>
       <c r="F40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M40" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.45">
@@ -28659,40 +28662,40 @@
         <v>15-64 (HIV+)</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>103</v>
       </c>
       <c r="G41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M41" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.45">
@@ -28701,40 +28704,40 @@
         <v>65+ (HIV+)</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G42" s="48" t="s">
         <v>103</v>
       </c>
       <c r="H42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M42" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.45">
@@ -28743,40 +28746,40 @@
         <v>Pris</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H43" s="48" t="s">
         <v>103</v>
       </c>
       <c r="I43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M43" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.45">
@@ -28785,40 +28788,40 @@
         <v>Pris (HIV+)</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I44" s="48" t="s">
         <v>103</v>
       </c>
       <c r="J44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M44" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.45">
@@ -28827,40 +28830,40 @@
         <v>HCW</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J45" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M45" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.45">
@@ -28869,40 +28872,40 @@
         <v>HCW (HIV+)</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K46" s="48" t="s">
         <v>103</v>
       </c>
       <c r="L46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M46" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.45">
@@ -28911,40 +28914,40 @@
         <v>Mine</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L47" s="48" t="s">
         <v>103</v>
       </c>
       <c r="M47" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.45">
@@ -28953,37 +28956,37 @@
         <v>Mine (HIV+)</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L48" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M48" s="48" t="s">
         <v>103</v>
@@ -29052,37 +29055,37 @@
         <v>103</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M51" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.45">
@@ -29091,40 +29094,40 @@
         <v>5-14</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C52" s="48" t="s">
         <v>103</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M52" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.45">
@@ -29133,40 +29136,40 @@
         <v>15-64</v>
       </c>
       <c r="B53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D53" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M53" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.45">
@@ -29175,40 +29178,40 @@
         <v>65+</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E54" s="48" t="s">
         <v>103</v>
       </c>
       <c r="F54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M54" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.45">
@@ -29217,40 +29220,40 @@
         <v>15-64 (HIV+)</v>
       </c>
       <c r="B55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>103</v>
       </c>
       <c r="G55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M55" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.45">
@@ -29259,40 +29262,40 @@
         <v>65+ (HIV+)</v>
       </c>
       <c r="B56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G56" s="48" t="s">
         <v>103</v>
       </c>
       <c r="H56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M56" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.45">
@@ -29301,40 +29304,40 @@
         <v>Pris</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H57" s="48" t="s">
         <v>103</v>
       </c>
       <c r="I57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M57" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.45">
@@ -29343,40 +29346,40 @@
         <v>Pris (HIV+)</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I58" s="48" t="s">
         <v>103</v>
       </c>
       <c r="J58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M58" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.45">
@@ -29385,40 +29388,40 @@
         <v>HCW</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J59" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M59" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.45">
@@ -29427,40 +29430,40 @@
         <v>HCW (HIV+)</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>103</v>
       </c>
       <c r="L60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M60" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.45">
@@ -29469,40 +29472,40 @@
         <v>Mine</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L61" s="48" t="s">
         <v>103</v>
       </c>
       <c r="M61" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.45">
@@ -29511,37 +29514,37 @@
         <v>Mine (HIV+)</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L62" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M62" s="48" t="s">
         <v>103</v>
@@ -29610,37 +29613,37 @@
         <v>103</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M65" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.45">
@@ -29649,40 +29652,40 @@
         <v>5-14</v>
       </c>
       <c r="B66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C66" s="48" t="s">
         <v>103</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M66" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.45">
@@ -29691,40 +29694,40 @@
         <v>15-64</v>
       </c>
       <c r="B67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D67" s="48" t="s">
         <v>103</v>
       </c>
       <c r="E67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M67" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.45">
@@ -29733,40 +29736,40 @@
         <v>65+</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E68" s="48" t="s">
         <v>103</v>
       </c>
       <c r="F68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M68" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.45">
@@ -29775,40 +29778,40 @@
         <v>15-64 (HIV+)</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>103</v>
       </c>
       <c r="G69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M69" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.45">
@@ -29817,40 +29820,40 @@
         <v>65+ (HIV+)</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G70" s="48" t="s">
         <v>103</v>
       </c>
       <c r="H70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M70" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.45">
@@ -29859,40 +29862,40 @@
         <v>Pris</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H71" s="48" t="s">
         <v>103</v>
       </c>
       <c r="I71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M71" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.45">
@@ -29901,40 +29904,40 @@
         <v>Pris (HIV+)</v>
       </c>
       <c r="B72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I72" s="48" t="s">
         <v>103</v>
       </c>
       <c r="J72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M72" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.45">
@@ -29943,40 +29946,40 @@
         <v>HCW</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J73" s="48" t="s">
         <v>103</v>
       </c>
       <c r="K73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M73" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.45">
@@ -29985,40 +29988,40 @@
         <v>HCW (HIV+)</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K74" s="48" t="s">
         <v>103</v>
       </c>
       <c r="L74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M74" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.45">
@@ -30027,40 +30030,40 @@
         <v>Mine</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L75" s="48" t="s">
         <v>103</v>
       </c>
       <c r="M75" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.45">
@@ -30069,37 +30072,37 @@
         <v>Mine (HIV+)</v>
       </c>
       <c r="B76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L76" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M76" s="48" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Handle deferred TDVE table import
Makes sure deferred time-dependent value entry tables can be read in, even though the transfer table is to be more complex.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A4E862-BD22-4EA6-AF1A-C38E200743F7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFD5D4D-198A-4101-B226-F0F40635493F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Transfer Definitions" sheetId="14" r:id="rId2"/>
-    <sheet name="Program Definitions" sheetId="2" r:id="rId3"/>
-    <sheet name="General Demographics" sheetId="3" r:id="rId4"/>
-    <sheet name="Active TB Prevalence" sheetId="4" r:id="rId5"/>
-    <sheet name="Latent TB Prevalence" sheetId="5" r:id="rId6"/>
-    <sheet name="Notified Cases" sheetId="6" r:id="rId7"/>
-    <sheet name="Infection Susceptibility" sheetId="7" r:id="rId8"/>
-    <sheet name="Latent Testing and Treatment" sheetId="8" r:id="rId9"/>
-    <sheet name="Latent Progression Rates" sheetId="9" r:id="rId10"/>
-    <sheet name="Active TB Testing and Treatment" sheetId="10" r:id="rId11"/>
-    <sheet name="Active TB Progression Rates" sheetId="11" r:id="rId12"/>
-    <sheet name="Active TB Death Rates" sheetId="12" r:id="rId13"/>
-    <sheet name="Metadata" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="Transfer Details" sheetId="15" r:id="rId3"/>
+    <sheet name="Program Definitions" sheetId="2" r:id="rId4"/>
+    <sheet name="General Demographics" sheetId="3" r:id="rId5"/>
+    <sheet name="Active TB Prevalence" sheetId="4" r:id="rId6"/>
+    <sheet name="Latent TB Prevalence" sheetId="5" r:id="rId7"/>
+    <sheet name="Notified Cases" sheetId="6" r:id="rId8"/>
+    <sheet name="Infection Susceptibility" sheetId="7" r:id="rId9"/>
+    <sheet name="Latent Testing and Treatment" sheetId="8" r:id="rId10"/>
+    <sheet name="Latent Progression Rates" sheetId="9" r:id="rId11"/>
+    <sheet name="Active TB Testing and Treatment" sheetId="10" r:id="rId12"/>
+    <sheet name="Active TB Progression Rates" sheetId="11" r:id="rId13"/>
+    <sheet name="Active TB Death Rates" sheetId="12" r:id="rId14"/>
+    <sheet name="Metadata" sheetId="13" state="hidden" r:id="rId15"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -73,6 +74,192 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000010000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000011000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000012000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000013000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000014000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000015000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -214,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -1280,7 +1467,7 @@
 </comments>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -1730,7 +1917,7 @@
 </comments>
 </file>
 
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -2331,6 +2518,286 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A6732E46-A56D-4C0B-AC5F-64483D7CAEBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{517EFC1F-2F1C-456C-9632-AA998818F13D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A41B63BD-24C2-4B9C-84A3-0DD9110F3045}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{35440989-D9A0-49CF-9D30-C97DF8D79C81}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{AB92BAAD-EBEA-49FE-9639-0E2FA42F22C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{E0307CEE-4603-4981-B78F-B9DBC2ABC6B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{E5654293-9522-42B1-A586-32F3A123B4BB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{0DA564C5-BEFE-4840-9237-5FE1B4445464}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{55E57EC2-1746-4E3D-A2D8-2B84BC921514}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{10AD02C1-ACF1-49E5-B8C5-EE493D69A34B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{20E04A99-E9A4-4DED-AF6D-293683DDB5F3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C43" authorId="0" shapeId="0" xr:uid="{C56E82D6-FC69-4454-86BB-0FF6BCB5DB7D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A57" authorId="0" shapeId="0" xr:uid="{6CC8A6EB-45D4-4E71-B433-698754019EF7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B57" authorId="0" shapeId="0" xr:uid="{5BC29C6A-3E43-483D-BB05-191111B4BCAB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C57" authorId="0" shapeId="0" xr:uid="{55E30D86-A8C0-4735-AFB8-889A68C3C7AE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
@@ -2365,7 +2832,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -2595,7 +3062,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -3573,7 +4040,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -3935,7 +4402,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -4297,7 +4764,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -4615,194 +5082,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000012000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000013000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000014000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="213">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -6537,6 +6818,1095 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:W55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="50.73046875" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="str">
+        <f>'Population Definitions'!B2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C13" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="78">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78">
+        <v>0.49289064565483448</v>
+      </c>
+      <c r="L2" s="78">
+        <v>0.4995</v>
+      </c>
+      <c r="M2" s="78">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="78">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="str">
+        <f>'Population Definitions'!B3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="str">
+        <f>'Population Definitions'!B4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="str">
+        <f>'Population Definitions'!B5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="str">
+        <f>'Population Definitions'!B6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="str">
+        <f>'Population Definitions'!B7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="str">
+        <f>'Population Definitions'!B8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="str">
+        <f>'Population Definitions'!B9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="str">
+        <f>'Population Definitions'!B10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="str">
+        <f>'Population Definitions'!B11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="str">
+        <f>'Population Definitions'!B12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="str">
+        <f>'Population Definitions'!B13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W15" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="str">
+        <f>'Population Definitions'!B2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C27" si="1">IF(SUMPRODUCT(--(E16:W16&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="str">
+        <f>'Population Definitions'!B3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="str">
+        <f>'Population Definitions'!B4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="str">
+        <f>'Population Definitions'!B5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="str">
+        <f>'Population Definitions'!B6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="str">
+        <f>'Population Definitions'!B7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="str">
+        <f>'Population Definitions'!B8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="str">
+        <f>'Population Definitions'!B9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="str">
+        <f>'Population Definitions'!B10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="str">
+        <f>'Population Definitions'!B11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="str">
+        <f>'Population Definitions'!B12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="str">
+        <f>'Population Definitions'!B13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P29" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R29" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S29" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T29" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U29" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W29" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="str">
+        <f>'Population Definitions'!B2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C41" si="2">IF(SUMPRODUCT(--(E30:W30&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="str">
+        <f>'Population Definitions'!B3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="str">
+        <f>'Population Definitions'!B4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="str">
+        <f>'Population Definitions'!B5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="str">
+        <f>'Population Definitions'!B6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="str">
+        <f>'Population Definitions'!B7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="str">
+        <f>'Population Definitions'!B8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="str">
+        <f>'Population Definitions'!B9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="str">
+        <f>'Population Definitions'!B10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="str">
+        <f>'Population Definitions'!B11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="str">
+        <f>'Population Definitions'!B12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="str">
+        <f>'Population Definitions'!B13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L43" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M43" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N43" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P43" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R43" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S43" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T43" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V43" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W43" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A44" s="2" t="str">
+        <f>'Population Definitions'!B2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:C55" si="3">IF(SUMPRODUCT(--(E44:W44&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="str">
+        <f>'Population Definitions'!B3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="str">
+        <f>'Population Definitions'!B4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="str">
+        <f>'Population Definitions'!B5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="str">
+        <f>'Population Definitions'!B6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="str">
+        <f>'Population Definitions'!B7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="str">
+        <f>'Population Definitions'!B8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" s="2" t="str">
+        <f>'Population Definitions'!B9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="str">
+        <f>'Population Definitions'!B10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" s="2" t="str">
+        <f>'Population Definitions'!B11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" s="2" t="str">
+        <f>'Population Definitions'!B12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" s="2" t="str">
+        <f>'Population Definitions'!B13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{00000000-0002-0000-0700-000024000000}">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55 B30:B41 B16:B27" xr:uid="{00000000-0002-0000-0700-000030000000}">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W41"/>
   <sheetViews>
@@ -7555,7 +8925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:W335"/>
   <sheetViews>
@@ -17442,7 +18812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:W139"/>
   <sheetViews>
@@ -20104,7 +21474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:W167"/>
   <sheetViews>
@@ -27207,7 +28577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -27248,7 +28618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A99255-0B6D-41A7-8133-CB3A9221CAB5}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -30123,6 +31493,1340 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B62B4-19B1-420D-9D4A-9272373B0398}">
+  <dimension ref="A1:W69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.19921875" style="143" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" style="143" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="143" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.06640625" style="143" bestFit="1" customWidth="1"/>
+    <col min="5" max="23" width="4.73046875" style="143" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.06640625" style="143"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="str">
+        <f>'Transfer Definitions'!B2</f>
+        <v>Aging</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A2" s="48" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="143">
+        <f t="shared" ref="C2:C13" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A3" s="48" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B3" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A4" s="48" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A5" s="48" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B5" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A6" s="48" t="str">
+        <f>'Population Definitions'!$B$6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B6" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A7" s="48" t="str">
+        <f>'Population Definitions'!$B$7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B7" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A8" s="48" t="str">
+        <f>'Population Definitions'!$B$8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B8" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A9" s="48" t="str">
+        <f>'Population Definitions'!$B$9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B9" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A10" s="48" t="str">
+        <f>'Population Definitions'!$B$10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B10" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A11" s="48" t="str">
+        <f>'Population Definitions'!$B$11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B11" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A12" s="48" t="str">
+        <f>'Population Definitions'!$B$12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B12" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A13" s="48" t="str">
+        <f>'Population Definitions'!$B$13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B13" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="143">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="str">
+        <f>'Transfer Definitions'!$B$3</f>
+        <v>HIV Infection</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W15" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A16" s="48" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B16" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="143">
+        <f t="shared" ref="C16:C27" si="1">IF(SUMPRODUCT(--(E16:W16&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A17" s="48" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B17" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A18" s="48" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B18" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A19" s="48" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B19" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A20" s="48" t="str">
+        <f>'Population Definitions'!$B$6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B20" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A21" s="48" t="str">
+        <f>'Population Definitions'!$B$7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B21" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A22" s="48" t="str">
+        <f>'Population Definitions'!$B$8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B22" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A23" s="48" t="str">
+        <f>'Population Definitions'!$B$9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B23" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A24" s="48" t="str">
+        <f>'Population Definitions'!$B$10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B24" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A25" s="48" t="str">
+        <f>'Population Definitions'!$B$11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B25" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A26" s="48" t="str">
+        <f>'Population Definitions'!$B$12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B26" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A27" s="48" t="str">
+        <f>'Population Definitions'!$B$13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B27" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="143">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="str">
+        <f>'Transfer Definitions'!$B$4</f>
+        <v>Transfer 2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P29" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R29" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S29" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T29" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U29" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W29" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A30" s="48" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B30" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="143">
+        <f t="shared" ref="C30:C41" si="2">IF(SUMPRODUCT(--(E30:W30&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A31" s="48" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B31" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A32" s="48" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B32" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A33" s="48" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B33" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A34" s="48" t="str">
+        <f>'Population Definitions'!$B$6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B34" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A35" s="48" t="str">
+        <f>'Population Definitions'!$B$7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B35" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A36" s="48" t="str">
+        <f>'Population Definitions'!$B$8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B36" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A37" s="48" t="str">
+        <f>'Population Definitions'!$B$9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B37" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A38" s="48" t="str">
+        <f>'Population Definitions'!$B$10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B38" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A39" s="48" t="str">
+        <f>'Population Definitions'!$B$11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B39" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A40" s="48" t="str">
+        <f>'Population Definitions'!$B$12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B40" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A41" s="48" t="str">
+        <f>'Population Definitions'!$B$13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B41" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="str">
+        <f>'Transfer Definitions'!$B$5</f>
+        <v>Transfer 3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L43" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M43" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N43" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P43" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R43" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S43" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T43" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V43" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W43" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A44" s="48" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B44" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="143">
+        <f t="shared" ref="C44:C55" si="3">IF(SUMPRODUCT(--(E44:W44&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A45" s="48" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B45" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A46" s="48" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B46" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A47" s="48" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B47" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A48" s="48" t="str">
+        <f>'Population Definitions'!$B$6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B48" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A49" s="48" t="str">
+        <f>'Population Definitions'!$B$7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B49" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A50" s="48" t="str">
+        <f>'Population Definitions'!$B$8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B50" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A51" s="48" t="str">
+        <f>'Population Definitions'!$B$9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B51" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A52" s="48" t="str">
+        <f>'Population Definitions'!$B$10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B52" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A53" s="48" t="str">
+        <f>'Population Definitions'!$B$11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B53" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A54" s="48" t="str">
+        <f>'Population Definitions'!$B$12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B54" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A55" s="48" t="str">
+        <f>'Population Definitions'!$B$13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B55" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="str">
+        <f>'Transfer Definitions'!$B$6</f>
+        <v>Transfer 4</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G57" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H57" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I57" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J57" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K57" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L57" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M57" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N57" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O57" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P57" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R57" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S57" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T57" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U57" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V57" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W57" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A58" s="48" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>Gen 0-4</v>
+      </c>
+      <c r="B58" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="143">
+        <f t="shared" ref="C58:C69" si="4">IF(SUMPRODUCT(--(E58:W58&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A59" s="48" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>Gen 5-14</v>
+      </c>
+      <c r="B59" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A60" s="48" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>Gen 15-64</v>
+      </c>
+      <c r="B60" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D60" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A61" s="48" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Gen 65+</v>
+      </c>
+      <c r="B61" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A62" s="48" t="str">
+        <f>'Population Definitions'!$B$6</f>
+        <v>PLHIV 15-64</v>
+      </c>
+      <c r="B62" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A63" s="48" t="str">
+        <f>'Population Definitions'!$B$7</f>
+        <v>PLHIV 65+</v>
+      </c>
+      <c r="B63" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D63" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A64" s="48" t="str">
+        <f>'Population Definitions'!$B$8</f>
+        <v>Prisoners</v>
+      </c>
+      <c r="B64" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D64" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65" s="48" t="str">
+        <f>'Population Definitions'!$B$9</f>
+        <v>PLHIV Prisoners</v>
+      </c>
+      <c r="B65" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D65" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66" s="48" t="str">
+        <f>'Population Definitions'!$B$10</f>
+        <v>Health Care Workers</v>
+      </c>
+      <c r="B66" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D66" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" s="48" t="str">
+        <f>'Population Definitions'!$B$11</f>
+        <v>PLHIV Health Care Workers</v>
+      </c>
+      <c r="B67" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D67" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68" s="48" t="str">
+        <f>'Population Definitions'!$B$12</f>
+        <v>Miners</v>
+      </c>
+      <c r="B68" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D68" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" s="48" t="str">
+        <f>'Population Definitions'!$B$13</f>
+        <v>PLHIV Miners</v>
+      </c>
+      <c r="B69" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D69" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58:B69 B44:B55 B30:B41 B16:B27 B2:B13" xr:uid="{0D430C7E-40F4-40CB-AAB0-E03DC5804038}">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -30395,7 +33099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W69"/>
   <sheetViews>
@@ -33219,7 +35923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W307"/>
   <sheetViews>
@@ -42089,7 +44793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W111"/>
   <sheetViews>
@@ -44298,7 +47002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W111"/>
   <sheetViews>
@@ -48945,7 +51649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:W97"/>
   <sheetViews>
@@ -50954,1093 +53658,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:W55"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="50.73046875" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Gen 0-4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C13" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="78">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78">
-        <v>0.49289064565483448</v>
-      </c>
-      <c r="L2" s="78">
-        <v>0.4995</v>
-      </c>
-      <c r="M2" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="N2" s="78">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="str">
-        <f>'Population Definitions'!B3</f>
-        <v>Gen 5-14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="str">
-        <f>'Population Definitions'!B4</f>
-        <v>Gen 15-64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="str">
-        <f>'Population Definitions'!B5</f>
-        <v>Gen 65+</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="str">
-        <f>'Population Definitions'!B6</f>
-        <v>PLHIV 15-64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="str">
-        <f>'Population Definitions'!B7</f>
-        <v>PLHIV 65+</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="str">
-        <f>'Population Definitions'!B8</f>
-        <v>Prisoners</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="str">
-        <f>'Population Definitions'!B9</f>
-        <v>PLHIV Prisoners</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="str">
-        <f>'Population Definitions'!B10</f>
-        <v>Health Care Workers</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="str">
-        <f>'Population Definitions'!B11</f>
-        <v>PLHIV Health Care Workers</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="str">
-        <f>'Population Definitions'!B12</f>
-        <v>Miners</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="str">
-        <f>'Population Definitions'!B13</f>
-        <v>PLHIV Miners</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H15" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I15" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J15" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K15" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L15" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M15" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N15" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O15" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P15" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R15" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S15" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T15" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U15" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V15" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W15" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Gen 0-4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C27" si="1">IF(SUMPRODUCT(--(E16:W16&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="str">
-        <f>'Population Definitions'!B3</f>
-        <v>Gen 5-14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="str">
-        <f>'Population Definitions'!B4</f>
-        <v>Gen 15-64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="str">
-        <f>'Population Definitions'!B5</f>
-        <v>Gen 65+</v>
-      </c>
-      <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="str">
-        <f>'Population Definitions'!B6</f>
-        <v>PLHIV 15-64</v>
-      </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="str">
-        <f>'Population Definitions'!B7</f>
-        <v>PLHIV 65+</v>
-      </c>
-      <c r="B21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="str">
-        <f>'Population Definitions'!B8</f>
-        <v>Prisoners</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="str">
-        <f>'Population Definitions'!B9</f>
-        <v>PLHIV Prisoners</v>
-      </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="str">
-        <f>'Population Definitions'!B10</f>
-        <v>Health Care Workers</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="str">
-        <f>'Population Definitions'!B11</f>
-        <v>PLHIV Health Care Workers</v>
-      </c>
-      <c r="B25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="str">
-        <f>'Population Definitions'!B12</f>
-        <v>Miners</v>
-      </c>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="str">
-        <f>'Population Definitions'!B13</f>
-        <v>PLHIV Miners</v>
-      </c>
-      <c r="B27" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G29" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I29" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J29" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K29" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L29" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M29" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N29" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O29" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P29" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R29" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S29" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T29" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U29" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V29" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W29" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Gen 0-4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30">
-        <f t="shared" ref="C30:C41" si="2">IF(SUMPRODUCT(--(E30:W30&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="str">
-        <f>'Population Definitions'!B3</f>
-        <v>Gen 5-14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="str">
-        <f>'Population Definitions'!B4</f>
-        <v>Gen 15-64</v>
-      </c>
-      <c r="B32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="str">
-        <f>'Population Definitions'!B5</f>
-        <v>Gen 65+</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="str">
-        <f>'Population Definitions'!B6</f>
-        <v>PLHIV 15-64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="str">
-        <f>'Population Definitions'!B7</f>
-        <v>PLHIV 65+</v>
-      </c>
-      <c r="B35" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="str">
-        <f>'Population Definitions'!B8</f>
-        <v>Prisoners</v>
-      </c>
-      <c r="B36" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="str">
-        <f>'Population Definitions'!B9</f>
-        <v>PLHIV Prisoners</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A38" s="2" t="str">
-        <f>'Population Definitions'!B10</f>
-        <v>Health Care Workers</v>
-      </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="str">
-        <f>'Population Definitions'!B11</f>
-        <v>PLHIV Health Care Workers</v>
-      </c>
-      <c r="B39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="str">
-        <f>'Population Definitions'!B12</f>
-        <v>Miners</v>
-      </c>
-      <c r="B40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="str">
-        <f>'Population Definitions'!B13</f>
-        <v>PLHIV Miners</v>
-      </c>
-      <c r="B41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F43" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G43" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H43" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I43" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J43" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K43" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L43" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M43" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N43" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O43" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P43" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R43" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S43" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T43" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U43" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V43" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W43" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A44" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Gen 0-4</v>
-      </c>
-      <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44">
-        <f t="shared" ref="C44:C55" si="3">IF(SUMPRODUCT(--(E44:W44&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A45" s="2" t="str">
-        <f>'Population Definitions'!B3</f>
-        <v>Gen 5-14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A46" s="2" t="str">
-        <f>'Population Definitions'!B4</f>
-        <v>Gen 15-64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A47" s="2" t="str">
-        <f>'Population Definitions'!B5</f>
-        <v>Gen 65+</v>
-      </c>
-      <c r="B47" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A48" s="2" t="str">
-        <f>'Population Definitions'!B6</f>
-        <v>PLHIV 15-64</v>
-      </c>
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" s="2" t="str">
-        <f>'Population Definitions'!B7</f>
-        <v>PLHIV 65+</v>
-      </c>
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" s="2" t="str">
-        <f>'Population Definitions'!B8</f>
-        <v>Prisoners</v>
-      </c>
-      <c r="B50" t="s">
-        <v>103</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" s="2" t="str">
-        <f>'Population Definitions'!B9</f>
-        <v>PLHIV Prisoners</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" s="2" t="str">
-        <f>'Population Definitions'!B10</f>
-        <v>Health Care Workers</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" s="2" t="str">
-        <f>'Population Definitions'!B11</f>
-        <v>PLHIV Health Care Workers</v>
-      </c>
-      <c r="B53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" s="2" t="str">
-        <f>'Population Definitions'!B12</f>
-        <v>Miners</v>
-      </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" s="2" t="str">
-        <f>'Population Definitions'!B13</f>
-        <v>PLHIV Miners</v>
-      </c>
-      <c r="B55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{00000000-0002-0000-0700-000024000000}">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55 B30:B41 B16:B27" xr:uid="{00000000-0002-0000-0700-000030000000}">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Transfer propagation to parset
Transfer data is now propagated from the databook into the parameter set.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7F466-2585-4DDE-A949-E995C24DE758}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5474D5D5-4842-4501-B1E8-11A7A65D6E36}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31499,8 +31499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F50E057-7920-429F-B282-34FA5E6D8F62}">
   <dimension ref="A1:Y669"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="T164" sqref="T164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31600,8 +31600,7 @@
         <v>67</v>
       </c>
       <c r="E2" s="143">
-        <f t="shared" ref="E2:E65" si="0">IF(SUMPRODUCT(--(G2:Y2&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F2" s="48" t="s">
         <v>68</v>
@@ -31623,7 +31622,7 @@
         <v>67</v>
       </c>
       <c r="E3" s="143">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E2:E65" si="0">IF(SUMPRODUCT(--(G3:Y3&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F3" s="48" t="s">
@@ -31876,8 +31875,7 @@
         <v>67</v>
       </c>
       <c r="E14" s="143">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F14" s="48" t="s">
         <v>68</v>
@@ -32152,8 +32150,7 @@
         <v>67</v>
       </c>
       <c r="E26" s="143">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>68</v>
@@ -34544,7 +34541,7 @@
         <v>67</v>
       </c>
       <c r="E130" s="143">
-        <f t="shared" ref="E130:E165" si="2">IF(SUMPRODUCT(--(G130:Y130&lt;&gt;""))=0,0,"N.A.")</f>
+        <f t="shared" ref="E130:E133" si="2">IF(SUMPRODUCT(--(G130:Y130&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F130" s="48" t="s">
@@ -35264,7 +35261,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A161" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35279,15 +35276,21 @@
       <c r="D161" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="E161" s="143">
+      <c r="E161" s="143" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="F161" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="L161" s="143">
+        <v>0.1</v>
+      </c>
+      <c r="Q161" s="143">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A162" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35310,7 +35313,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A163" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35333,7 +35336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A164" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35356,7 +35359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A165" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35379,7 +35382,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A166" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35402,7 +35405,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A167" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35425,7 +35428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A168" s="48" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>Gen 15-64</v>
@@ -35448,7 +35451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A169" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35471,7 +35474,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A170" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35494,7 +35497,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A171" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35517,7 +35520,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A172" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35540,7 +35543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A173" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35555,15 +35558,21 @@
       <c r="D173" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="E173" s="143">
+      <c r="E173" s="143" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="F173" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="N173" s="143">
+        <v>0.15</v>
+      </c>
+      <c r="U173" s="143">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A174" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35586,7 +35595,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A175" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -35609,7 +35618,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A176" s="48" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Gen 65+</v>
@@ -37649,7 +37658,7 @@
         <v>67</v>
       </c>
       <c r="E264" s="143">
-        <f t="shared" ref="E264:E299" si="5">IF(SUMPRODUCT(--(G264:Y264&lt;&gt;""))=0,0,"N.A.")</f>
+        <f t="shared" ref="E264:E267" si="5">IF(SUMPRODUCT(--(G264:Y264&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F264" s="48" t="s">
@@ -40754,7 +40763,7 @@
         <v>67</v>
       </c>
       <c r="E398" s="143">
-        <f t="shared" ref="E398:E433" si="8">IF(SUMPRODUCT(--(G398:Y398&lt;&gt;""))=0,0,"N.A.")</f>
+        <f t="shared" ref="E398:E401" si="8">IF(SUMPRODUCT(--(G398:Y398&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F398" s="48" t="s">
@@ -43859,7 +43868,7 @@
         <v>67</v>
       </c>
       <c r="E532" s="143">
-        <f t="shared" ref="E532:E567" si="11">IF(SUMPRODUCT(--(G532:Y532&lt;&gt;""))=0,0,"N.A.")</f>
+        <f t="shared" ref="E532:E535" si="11">IF(SUMPRODUCT(--(G532:Y532&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F532" s="48" t="s">
@@ -46964,7 +46973,7 @@
         <v>67</v>
       </c>
       <c r="E666" s="143">
-        <f t="shared" ref="E666:E701" si="14">IF(SUMPRODUCT(--(G666:Y666&lt;&gt;""))=0,0,"N.A.")</f>
+        <f t="shared" ref="E666:E669" si="14">IF(SUMPRODUCT(--(G666:Y666&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="F666" s="48" t="s">

</xml_diff>

<commit_message>
Working routines to add/remove interactions
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF55C73F-C45D-41F0-8889-4D4383D6195B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDE8F85-F275-479C-8E78-44CAFD7B02DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -4794,7 +4794,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4631" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="167">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -5289,6 +5289,12 @@
   </si>
   <si>
     <t>MDR-SN treatment success rate</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
 </sst>
 </file>
@@ -26698,10 +26704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B59E2B-8AEE-414D-930F-8BD277BF9EDB}">
-  <dimension ref="A1:W488"/>
+  <dimension ref="A1:Y488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y274" sqref="Y274"/>
+    <sheetView topLeftCell="A480" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U497" sqref="U497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27283,7 +27289,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -27345,8 +27351,14 @@
       <c r="W18" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f>IF($B$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27382,7 +27394,7 @@
       <c r="V19" s="165"/>
       <c r="W19" s="165"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f>IF($C$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>0-4</v>
@@ -27433,7 +27445,7 @@
       <c r="V20" s="165"/>
       <c r="W20" s="165"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>IF($D$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27469,7 +27481,7 @@
       <c r="V21" s="165"/>
       <c r="W21" s="165"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f>IF($E$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27505,7 +27517,7 @@
       <c r="V22" s="165"/>
       <c r="W22" s="165"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f>IF($F$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27541,7 +27553,7 @@
       <c r="V23" s="165"/>
       <c r="W23" s="165"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f>IF($G$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27577,7 +27589,7 @@
       <c r="V24" s="165"/>
       <c r="W24" s="165"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f>IF($H$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27613,7 +27625,7 @@
       <c r="V25" s="165"/>
       <c r="W25" s="165"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f>IF($I$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27649,7 +27661,7 @@
       <c r="V26" s="165"/>
       <c r="W26" s="165"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f>IF($J$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27685,7 +27697,7 @@
       <c r="V27" s="165"/>
       <c r="W27" s="165"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f>IF($K$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27721,7 +27733,7 @@
       <c r="V28" s="165"/>
       <c r="W28" s="165"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f>IF($L$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27757,7 +27769,7 @@
       <c r="V29" s="165"/>
       <c r="W29" s="165"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
         <f>IF($M$5="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -27793,7 +27805,7 @@
       <c r="V30" s="165"/>
       <c r="W30" s="165"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
         <f>IF($B$6="Y",'[1]Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -27829,7 +27841,7 @@
       <c r="V31" s="165"/>
       <c r="W31" s="165"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
         <f>IF($C$6="Y",'[1]Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -33054,7 +33066,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="str">
         <f>'[1]Population Definitions'!$A$11</f>
         <v>HCW (HIV+)</v>
@@ -33096,7 +33108,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="str">
         <f>'[1]Population Definitions'!$A$12</f>
         <v>Mine</v>
@@ -33138,7 +33150,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="str">
         <f>'[1]Population Definitions'!$A$13</f>
         <v>Mine (HIV+)</v>
@@ -33180,7 +33192,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -33242,8 +33254,14 @@
       <c r="W181" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X181" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y181" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="str">
         <f>IF($B$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33279,7 +33297,7 @@
       <c r="V182" s="165"/>
       <c r="W182" s="165"/>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="str">
         <f>IF($C$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33315,7 +33333,7 @@
       <c r="V183" s="165"/>
       <c r="W183" s="165"/>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="str">
         <f>IF($D$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33351,7 +33369,7 @@
       <c r="V184" s="165"/>
       <c r="W184" s="165"/>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="str">
         <f>IF($E$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33387,7 +33405,7 @@
       <c r="V185" s="165"/>
       <c r="W185" s="165"/>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="str">
         <f>IF($F$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33423,7 +33441,7 @@
       <c r="V186" s="165"/>
       <c r="W186" s="165"/>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="str">
         <f>IF($G$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33459,7 +33477,7 @@
       <c r="V187" s="165"/>
       <c r="W187" s="165"/>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="str">
         <f>IF($H$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33495,7 +33513,7 @@
       <c r="V188" s="165"/>
       <c r="W188" s="165"/>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="str">
         <f>IF($I$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33531,7 +33549,7 @@
       <c r="V189" s="165"/>
       <c r="W189" s="165"/>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="str">
         <f>IF($J$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33567,7 +33585,7 @@
       <c r="V190" s="165"/>
       <c r="W190" s="165"/>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="str">
         <f>IF($K$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -33603,7 +33621,7 @@
       <c r="V191" s="165"/>
       <c r="W191" s="165"/>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="str">
         <f>IF($L$168="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -38878,7 +38896,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="337" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="str">
         <f>'[1]Population Definitions'!$A$8</f>
         <v>Pris</v>
@@ -38920,7 +38938,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="338" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="str">
         <f>'[1]Population Definitions'!$A$9</f>
         <v>Pris (HIV+)</v>
@@ -38962,7 +38980,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="339" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="str">
         <f>'[1]Population Definitions'!$A$10</f>
         <v>HCW</v>
@@ -39004,7 +39022,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="340" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="str">
         <f>'[1]Population Definitions'!$A$11</f>
         <v>HCW (HIV+)</v>
@@ -39046,7 +39064,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="341" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="str">
         <f>'[1]Population Definitions'!$A$12</f>
         <v>Mine</v>
@@ -39088,7 +39106,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="342" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="str">
         <f>'[1]Population Definitions'!$A$13</f>
         <v>Mine (HIV+)</v>
@@ -39130,7 +39148,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="344" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -39192,8 +39210,14 @@
       <c r="W344" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="345" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X344" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y344" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="str">
         <f>IF($B$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39229,7 +39253,7 @@
       <c r="V345" s="165"/>
       <c r="W345" s="165"/>
     </row>
-    <row r="346" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="str">
         <f>IF($C$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39265,7 +39289,7 @@
       <c r="V346" s="165"/>
       <c r="W346" s="165"/>
     </row>
-    <row r="347" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="str">
         <f>IF($D$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39301,7 +39325,7 @@
       <c r="V347" s="165"/>
       <c r="W347" s="165"/>
     </row>
-    <row r="348" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="str">
         <f>IF($E$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39337,7 +39361,7 @@
       <c r="V348" s="165"/>
       <c r="W348" s="165"/>
     </row>
-    <row r="349" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="str">
         <f>IF($F$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39373,7 +39397,7 @@
       <c r="V349" s="165"/>
       <c r="W349" s="165"/>
     </row>
-    <row r="350" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="str">
         <f>IF($G$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39409,7 +39433,7 @@
       <c r="V350" s="165"/>
       <c r="W350" s="165"/>
     </row>
-    <row r="351" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="str">
         <f>IF($H$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -39445,7 +39469,7 @@
       <c r="V351" s="165"/>
       <c r="W351" s="165"/>
     </row>
-    <row r="352" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="str">
         <f>IF($I$331="Y",'[1]Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -44598,7 +44622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66525F71-991B-4C29-A0F4-FC0107D81B44}">
   <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed sheets on new databooks
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FEFB43-9187-4FFC-9C62-9F8D4B6DD699}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428B19AA-9062-4B0D-87E2-B7CC0FE3AFD2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
-    <sheet name="Transfers" sheetId="19" r:id="rId2"/>
-    <sheet name="Interactions" sheetId="18" r:id="rId3"/>
-    <sheet name="General Demographics" sheetId="3" r:id="rId4"/>
-    <sheet name="Active TB Prevalence" sheetId="4" r:id="rId5"/>
-    <sheet name="Latent TB Prevalence" sheetId="5" r:id="rId6"/>
-    <sheet name="Notified Cases" sheetId="6" r:id="rId7"/>
-    <sheet name="Infection Susceptibility" sheetId="7" r:id="rId8"/>
-    <sheet name="Latent Testing and Treatment" sheetId="8" r:id="rId9"/>
-    <sheet name="Latent Progression Rates" sheetId="9" r:id="rId10"/>
-    <sheet name="Active TB Testing and Treatment" sheetId="10" r:id="rId11"/>
-    <sheet name="Active TB Progression Rates" sheetId="11" r:id="rId12"/>
-    <sheet name="Active TB Death Rates" sheetId="12" r:id="rId13"/>
+    <sheet name="#ignore Extra" sheetId="20" r:id="rId1"/>
+    <sheet name="Population Definitions" sheetId="1" r:id="rId2"/>
+    <sheet name="Transfers" sheetId="19" r:id="rId3"/>
+    <sheet name="Interactions" sheetId="18" r:id="rId4"/>
+    <sheet name="General Demographics" sheetId="3" r:id="rId5"/>
+    <sheet name="Active TB Prevalence" sheetId="4" r:id="rId6"/>
+    <sheet name="Latent TB Prevalence" sheetId="5" r:id="rId7"/>
+    <sheet name="Notified Cases" sheetId="6" r:id="rId8"/>
+    <sheet name="Infection Susceptibility" sheetId="7" r:id="rId9"/>
+    <sheet name="Latent Testing and Treatment" sheetId="8" r:id="rId10"/>
+    <sheet name="Latent Progression Rates" sheetId="9" r:id="rId11"/>
+    <sheet name="Active TB Testing and Treatment" sheetId="10" r:id="rId12"/>
+    <sheet name="Active TB Progression Rates" sheetId="11" r:id="rId13"/>
+    <sheet name="Active TB Death Rates" sheetId="12" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="179017"/>
 </workbook>
@@ -4819,7 +4820,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4640" uniqueCount="170">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -5326,6 +5327,9 @@
   </si>
   <si>
     <t>This is a new cell</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -6445,138 +6449,1081 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FC0954-BED7-40C6-9B08-5D5840A56976}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>x</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:W55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="165" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C13" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="67">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F2" s="67">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G2" s="67">
+        <v>0</v>
+      </c>
+      <c r="H2" s="67">
+        <v>0</v>
+      </c>
+      <c r="I2" s="67">
+        <v>0</v>
+      </c>
+      <c r="J2" s="67">
+        <v>0</v>
+      </c>
+      <c r="K2" s="67">
+        <v>0.49289064565483448</v>
+      </c>
+      <c r="L2" s="67">
+        <v>0.4995</v>
+      </c>
+      <c r="M2" s="67">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="67">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="165" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="165" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="165" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="165" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="165" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="165" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="165" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="165" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="165" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="165" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="165" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W15" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="165" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="166" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C27" si="1">IF(SUMPRODUCT(--(E16:W16&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="166" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="165" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="166" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="165" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="166" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="165" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="166" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="165" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="166" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="165" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="166" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="165" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="166" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="165" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="166" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="165" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="166" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="165" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="166" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="165" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="166" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="166" t="s">
-        <v>168</v>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P29" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R29" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S29" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T29" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U29" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W29" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="165" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C41" si="2">IF(SUMPRODUCT(--(E30:W30&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="165" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="165" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="165" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="165" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="165" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="165" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="165" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="165" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="165" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="165" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="165" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2002</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2003</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2004</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2005</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2006</v>
+      </c>
+      <c r="L43" s="1">
+        <v>2007</v>
+      </c>
+      <c r="M43" s="1">
+        <v>2008</v>
+      </c>
+      <c r="N43" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2010</v>
+      </c>
+      <c r="P43" s="1">
+        <v>2011</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>2012</v>
+      </c>
+      <c r="R43" s="1">
+        <v>2013</v>
+      </c>
+      <c r="S43" s="1">
+        <v>2014</v>
+      </c>
+      <c r="T43" s="1">
+        <v>2015</v>
+      </c>
+      <c r="U43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="V43" s="1">
+        <v>2017</v>
+      </c>
+      <c r="W43" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="165" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:C55" si="3">IF(SUMPRODUCT(--(E44:W44&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="165" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="165" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="165" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" s="165" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="165" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="165" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="165" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="165" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="165" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="165" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="165" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{00000000-0002-0000-0700-000024000000}">
+      <formula1>"Number,Probability"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55 B30:B41 B16:B27" xr:uid="{00000000-0002-0000-0700-000030000000}">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W41"/>
   <sheetViews>
@@ -7459,7 +8406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:W335"/>
   <sheetViews>
@@ -17061,7 +18008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:W139"/>
   <sheetViews>
@@ -19603,7 +20550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:W167"/>
   <sheetViews>
@@ -26767,6 +27714,138 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="166" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="166" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="166" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="166" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="166" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="166" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="166" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="166" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="166" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="166" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="166" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="166" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="167" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="166" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B59E2B-8AEE-414D-930F-8BD277BF9EDB}">
   <dimension ref="A1:Y488"/>
   <sheetViews>
@@ -44682,7 +45761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66525F71-991B-4C29-A0F4-FC0107D81B44}">
   <dimension ref="A1:Y162"/>
   <sheetViews>
@@ -48933,7 +50012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W69"/>
   <sheetViews>
@@ -51795,7 +52874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W307"/>
   <sheetViews>
@@ -60401,7 +61480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W111"/>
   <sheetViews>
@@ -62540,7 +63619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W111"/>
   <sheetViews>
@@ -66806,7 +67885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:W97"/>
   <sheetViews>
@@ -68496,1055 +69575,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:W55"/>
-  <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C13" si="0">IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="67">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="F2" s="67">
-        <v>0</v>
-      </c>
-      <c r="G2" s="67">
-        <v>0</v>
-      </c>
-      <c r="H2" s="67">
-        <v>0</v>
-      </c>
-      <c r="I2" s="67">
-        <v>0</v>
-      </c>
-      <c r="J2" s="67">
-        <v>0</v>
-      </c>
-      <c r="K2" s="67">
-        <v>0.49289064565483448</v>
-      </c>
-      <c r="L2" s="67">
-        <v>0.4995</v>
-      </c>
-      <c r="M2" s="67">
-        <v>0.5</v>
-      </c>
-      <c r="N2" s="67">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="165" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="165" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="165" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="165" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="165" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="165" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="165" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="165" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="165" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H15" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I15" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J15" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K15" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L15" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M15" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N15" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O15" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P15" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R15" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S15" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T15" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U15" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V15" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W15" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="165" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C27" si="1">IF(SUMPRODUCT(--(E16:W16&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="165" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="165" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="165" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="165" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="165" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="165" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="165" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="165" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="165" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G29" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I29" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J29" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K29" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L29" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M29" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N29" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O29" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P29" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R29" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S29" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T29" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U29" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V29" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W29" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="165" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30">
-        <f t="shared" ref="C30:C41" si="2">IF(SUMPRODUCT(--(E30:W30&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="165" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="165" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="165" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="165" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="165" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" s="165" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="165" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="165" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="165" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F43" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G43" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H43" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I43" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J43" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K43" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L43" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M43" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N43" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O43" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P43" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R43" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S43" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T43" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U43" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V43" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W43" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="165" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44">
-        <f t="shared" ref="C44:C55" si="3">IF(SUMPRODUCT(--(E44:W44&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="165" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="165" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="165" t="s">
-        <v>119</v>
-      </c>
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="165" t="s">
-        <v>121</v>
-      </c>
-      <c r="B49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="165" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="165" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="165" t="s">
-        <v>124</v>
-      </c>
-      <c r="B52" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="B53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="165" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="165" t="s">
-        <v>131</v>
-      </c>
-      <c r="B55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13" xr:uid="{00000000-0002-0000-0700-000024000000}">
-      <formula1>"Number,Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55 B30:B41 B16:B27" xr:uid="{00000000-0002-0000-0700-000030000000}">
-      <formula1>"N.A."</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ok, lets go with this
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_tb.xlsx
+++ b/tests/databooks/databook_tb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -5295,7 +5295,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="10">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
@@ -5460,7 +5461,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5938,6 +5939,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -26665,7 +26667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
@@ -30570,8 +30572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30668,7 +30670,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="36">
-        <v>1628.791055731323</v>
+        <v>276.89447947432495</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -30686,8 +30688,9 @@
         <v>6</v>
       </c>
       <c r="E3" s="36">
-        <v>724.8636958939444</v>
-      </c>
+        <v>123.22682830197056</v>
+      </c>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="165" t="s">
@@ -30704,8 +30707,9 @@
         <v>6</v>
       </c>
       <c r="E4" s="36">
-        <v>2536.7679116949062</v>
-      </c>
+        <v>431.2505449881341</v>
+      </c>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="165" t="s">
@@ -30722,8 +30726,9 @@
         <v>6</v>
       </c>
       <c r="E5" s="36">
-        <v>174.95334850864231</v>
-      </c>
+        <v>29.742069246469196</v>
+      </c>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="165" t="s">
@@ -30740,8 +30745,9 @@
         <v>6</v>
       </c>
       <c r="E6" s="36">
-        <v>13686.100331738851</v>
-      </c>
+        <v>2326.6370563956048</v>
+      </c>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="165" t="s">
@@ -30758,8 +30764,9 @@
         <v>6</v>
       </c>
       <c r="E7" s="36">
-        <v>82.136361286302488</v>
-      </c>
+        <v>13.963181418671423</v>
+      </c>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="165" t="s">
@@ -30776,8 +30783,9 @@
         <v>6</v>
       </c>
       <c r="E8" s="36">
-        <v>43.693093756809269</v>
-      </c>
+        <v>7.427825938657576</v>
+      </c>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="165" t="s">
@@ -30794,8 +30802,9 @@
         <v>6</v>
       </c>
       <c r="E9" s="36">
-        <v>243.56028604774679</v>
-      </c>
+        <v>41.405248628116958</v>
+      </c>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="165" t="s">
@@ -32256,7 +32265,7 @@
         <v>6</v>
       </c>
       <c r="E86" s="29">
-        <v>264.09966401000003</v>
+        <v>448.96942881700005</v>
       </c>
     </row>
     <row r="87" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -32274,8 +32283,9 @@
         <v>6</v>
       </c>
       <c r="E87" s="29">
-        <v>1378.1346600000002</v>
-      </c>
+        <v>2342.8289220000001</v>
+      </c>
+      <c r="F87" s="131"/>
     </row>
     <row r="88" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="165" t="s">
@@ -32292,8 +32302,9 @@
         <v>6</v>
       </c>
       <c r="E88" s="29">
-        <v>7643.2497136800012</v>
-      </c>
+        <v>12993.524513256001</v>
+      </c>
+      <c r="F88" s="131"/>
     </row>
     <row r="89" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="165" t="s">
@@ -32310,8 +32321,9 @@
         <v>6</v>
       </c>
       <c r="E89" s="29">
-        <v>870.52809795000007</v>
-      </c>
+        <v>1479.8977665150001</v>
+      </c>
+      <c r="F89" s="131"/>
     </row>
     <row r="90" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="165" t="s">
@@ -32328,8 +32340,9 @@
         <v>6</v>
       </c>
       <c r="E90" s="29">
-        <v>41037.760542999997</v>
-      </c>
+        <v>69764.192923099996</v>
+      </c>
+      <c r="F90" s="131"/>
     </row>
     <row r="91" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="165" t="s">
@@ -32346,8 +32359,9 @@
         <v>6</v>
       </c>
       <c r="E91" s="29">
-        <v>400.52177424000001</v>
-      </c>
+        <v>680.88701620799998</v>
+      </c>
+      <c r="F91" s="131"/>
     </row>
     <row r="92" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="165" t="s">
@@ -32364,8 +32378,9 @@
         <v>6</v>
       </c>
       <c r="E92" s="29">
-        <v>504.51775107499998</v>
-      </c>
+        <v>857.68017682749996</v>
+      </c>
+      <c r="F92" s="131"/>
     </row>
     <row r="93" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="165" t="s">
@@ -32382,8 +32397,9 @@
         <v>6</v>
       </c>
       <c r="E93" s="29">
-        <v>494.37069438461538</v>
-      </c>
+        <v>840.43018045384611</v>
+      </c>
+      <c r="F93" s="131"/>
     </row>
     <row r="94" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="165" t="s">
@@ -39176,8 +39192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W111"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:A111"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39187,7 +39203,8 @@
     <col min="3" max="3" width="10.7109375" style="35" customWidth="1"/>
     <col min="4" max="4" width="9" style="35"/>
     <col min="5" max="5" width="9.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="35"/>
+    <col min="6" max="6" width="10.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -39273,11 +39290,12 @@
         <v>6</v>
       </c>
       <c r="E2" s="38">
-        <v>196086.5355</v>
+        <v>333347.11034999997</v>
       </c>
       <c r="F2" s="38">
-        <v>345769.89500000002</v>
-      </c>
+        <v>587808.82149999996</v>
+      </c>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="165" t="s">
@@ -39294,11 +39312,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="38">
-        <v>20108.095701425736</v>
+        <v>34183.762692423748</v>
       </c>
       <c r="F3" s="38">
-        <v>20571.5493687784</v>
-      </c>
+        <v>34971.633926923278</v>
+      </c>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="165" t="s">
@@ -39315,9 +39335,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="38">
-        <v>549888.96905186586</v>
-      </c>
-      <c r="F4" s="38"/>
+        <v>934811.24738817196</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0</v>
+      </c>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="165" t="s">
@@ -39537,9 +39561,9 @@
         <v>6</v>
       </c>
       <c r="E16" s="41">
-        <v>11989.172171602127</v>
-      </c>
-      <c r="F16" s="161"/>
+        <v>20381.592691723617</v>
+      </c>
+      <c r="F16" s="166"/>
       <c r="H16" s="54"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -39557,9 +39581,9 @@
         <v>6</v>
       </c>
       <c r="E17" s="41">
-        <v>940.57531764110195</v>
-      </c>
-      <c r="F17" s="161"/>
+        <v>1598.9780399898732</v>
+      </c>
+      <c r="F17" s="166"/>
       <c r="H17" s="54"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -39577,9 +39601,9 @@
         <v>6</v>
       </c>
       <c r="E18" s="41">
-        <v>111046.39073066738</v>
-      </c>
-      <c r="F18" s="161"/>
+        <v>188778.86424213453</v>
+      </c>
+      <c r="F18" s="166"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="165" t="s">
@@ -39596,9 +39620,9 @@
         <v>6</v>
       </c>
       <c r="E19" s="41">
-        <v>559.0348756011075</v>
-      </c>
-      <c r="F19" s="161"/>
+        <v>950.35928852188272</v>
+      </c>
+      <c r="F19" s="166"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="165" t="s">
@@ -39615,9 +39639,9 @@
         <v>6</v>
       </c>
       <c r="E20" s="41">
-        <v>25642.40270181272</v>
-      </c>
-      <c r="F20" s="161"/>
+        <v>43592.084593081621</v>
+      </c>
+      <c r="F20" s="166"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="165" t="s">
@@ -39634,9 +39658,9 @@
         <v>6</v>
       </c>
       <c r="E21" s="41">
-        <v>115.26492280435555</v>
-      </c>
-      <c r="F21" s="161"/>
+        <v>195.95036876740443</v>
+      </c>
+      <c r="F21" s="166"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="165" t="s">
@@ -39653,9 +39677,9 @@
         <v>6</v>
       </c>
       <c r="E22" s="41">
-        <v>3168.1275594077397</v>
-      </c>
-      <c r="F22" s="161"/>
+        <v>5385.8168509931575</v>
+      </c>
+      <c r="F22" s="166"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="165" t="s">
@@ -39672,9 +39696,9 @@
         <v>6</v>
       </c>
       <c r="E23" s="41">
-        <v>429.96016877676465</v>
-      </c>
-      <c r="F23" s="161"/>
+        <v>730.93228692049991</v>
+      </c>
+      <c r="F23" s="166"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="165" t="s">
@@ -39691,9 +39715,9 @@
         <v>6</v>
       </c>
       <c r="E24" s="41">
-        <v>884.22498996991453</v>
-      </c>
-      <c r="F24" s="161"/>
+        <v>1503.1824829488546</v>
+      </c>
+      <c r="F24" s="166"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="165" t="s">
@@ -39710,9 +39734,9 @@
         <v>6</v>
       </c>
       <c r="E25" s="41">
-        <v>1567.1981776765374</v>
-      </c>
-      <c r="F25" s="161"/>
+        <v>2664.2369020501137</v>
+      </c>
+      <c r="F25" s="166"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="165" t="s">
@@ -39729,9 +39753,9 @@
         <v>6</v>
       </c>
       <c r="E26" s="41">
-        <v>324.67907887243854</v>
-      </c>
-      <c r="F26" s="161"/>
+        <v>551.95443408314554</v>
+      </c>
+      <c r="F26" s="166"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="165" t="s">
@@ -39748,9 +39772,9 @@
         <v>6</v>
       </c>
       <c r="E27" s="41">
-        <v>66.73784880410004</v>
-      </c>
-      <c r="F27" s="161"/>
+        <v>113.45434296697006</v>
+      </c>
+      <c r="F27" s="166"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -40083,7 +40107,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="42">
-        <v>107902.54954441913</v>
+        <v>183434.33422551252</v>
       </c>
       <c r="F44" s="161"/>
     </row>
@@ -40102,7 +40126,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="42">
-        <v>8465.1778587699173</v>
+        <v>14390.802359908859</v>
       </c>
       <c r="F45" s="161"/>
     </row>
@@ -40121,7 +40145,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="42">
-        <v>1277033.4934026748</v>
+        <v>2170956.9387845472</v>
       </c>
       <c r="F46" s="161"/>
     </row>
@@ -40140,7 +40164,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="42">
-        <v>5031.3138804099681</v>
+        <v>8553.2335966969458</v>
       </c>
       <c r="F47" s="161"/>
     </row>
@@ -40159,7 +40183,7 @@
         <v>6</v>
       </c>
       <c r="E48" s="42">
-        <v>230781.62431631447</v>
+        <v>392328.76133773458</v>
       </c>
       <c r="F48" s="161"/>
     </row>
@@ -40178,7 +40202,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="42">
-        <v>1037.3843052391999</v>
+        <v>1763.5533189066398</v>
       </c>
       <c r="F49" s="161"/>
     </row>
@@ -40197,7 +40221,7 @@
         <v>6</v>
       </c>
       <c r="E50" s="42">
-        <v>7392.2976386180599</v>
+        <v>12566.905985650701</v>
       </c>
       <c r="F50" s="161"/>
     </row>
@@ -40216,7 +40240,7 @@
         <v>6</v>
       </c>
       <c r="E51" s="42">
-        <v>2436.4409564016664</v>
+        <v>4141.9496258828331</v>
       </c>
       <c r="F51" s="161"/>
     </row>
@@ -40235,7 +40259,7 @@
         <v>6</v>
       </c>
       <c r="E52" s="42">
-        <v>7958.0249097292308</v>
+        <v>13528.642346539693</v>
       </c>
       <c r="F52" s="161"/>
     </row>
@@ -40254,7 +40278,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="42">
-        <v>1044.7987851176918</v>
+        <v>1776.1579347000759</v>
       </c>
       <c r="F53" s="161"/>
     </row>
@@ -40273,7 +40297,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="42">
-        <v>2922.1117098519467</v>
+        <v>4967.5899067483097</v>
       </c>
       <c r="F54" s="161"/>
     </row>
@@ -40292,7 +40316,7 @@
         <v>6</v>
       </c>
       <c r="E55" s="42">
-        <v>600.64063923690037</v>
+        <v>1021.0890867027306</v>
       </c>
       <c r="F55" s="161"/>
     </row>

</xml_diff>